<commit_message>
Added error row handling
</commit_message>
<xml_diff>
--- a/Data/ConsolidatedPriceAudit.xlsx
+++ b/Data/ConsolidatedPriceAudit.xlsx
@@ -12,8 +12,9 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
-    <sheet name="Consolidated" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Faulty Rows" sheetId="3" r:id="rId1"/>
+    <sheet name="Consolidated" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>Fiscal Period</t>
   </si>
@@ -417,6 +418,51 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>